<commit_message>
18.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/March/18.03.2020 Requisition of Mughdo Corporation.xlsx
+++ b/2020/Requisition/March/18.03.2020 Requisition of Mughdo Corporation.xlsx
@@ -1084,7 +1084,7 @@
       <pane xSplit="4" ySplit="13" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F104" sqref="F104"/>
+      <selection pane="bottomRight" activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -4594,7 +4594,7 @@
         <v>21</v>
       </c>
       <c r="C103" s="21">
-        <v>500000</v>
+        <v>520000</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>132</v>
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C107" s="22">
         <f>SUBTOTAL(9,C102:C106)</f>
-        <v>500000</v>
+        <v>520000</v>
       </c>
       <c r="D107" s="15"/>
       <c r="E107" s="23"/>

</xml_diff>